<commit_message>
minor fixes and TODO added
</commit_message>
<xml_diff>
--- a/assets/rumhowler_data.xlsx
+++ b/assets/rumhowler_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\OneDrive\Työpöytä\Programming projects\alko_app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C31A6E-6B04-4A3F-B28E-71B211480228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E927FA-7B6D-4493-BBDE-DC01C7EC9267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="405">
   <si>
     <t>Rum</t>
   </si>
@@ -1169,6 +1169,72 @@
   </si>
   <si>
     <t>therumhowlerblog.com</t>
+  </si>
+  <si>
+    <t>Baltic Dark muovipullo</t>
+  </si>
+  <si>
+    <t>Rhum Negrita Dark Signature</t>
+  </si>
+  <si>
+    <t>Barra Oak Bay Dark</t>
+  </si>
+  <si>
+    <t>Ron Cabana Blanco muovipullo</t>
+  </si>
+  <si>
+    <t>Rhum Negrita White Signature</t>
+  </si>
+  <si>
+    <t>Propeller Dark Rum</t>
+  </si>
+  <si>
+    <t>Baltic Light muovipullo</t>
+  </si>
+  <si>
+    <t>Rommiviina muovipullo</t>
+  </si>
+  <si>
+    <t>Old Pascas Dark</t>
+  </si>
+  <si>
+    <t>Barra Oak Bay Dark muovipullo</t>
+  </si>
+  <si>
+    <t>Rhum Negrita Dark Signature muovipullo</t>
+  </si>
+  <si>
+    <t>Barceló Blanco Añejado</t>
+  </si>
+  <si>
+    <t>Ching Shih Dark Spiced</t>
+  </si>
+  <si>
+    <t>Barbados Rommi muovipullo</t>
+  </si>
+  <si>
+    <t>Barra Oak Bay White muovipullo</t>
+  </si>
+  <si>
+    <t>Negrita Spiced Golden</t>
+  </si>
+  <si>
+    <t>Ripa's Honey &amp; Chili</t>
+  </si>
+  <si>
+    <t>Planteray O.F.T.D</t>
+  </si>
+  <si>
+    <t>Bacardi Carta Negra</t>
+  </si>
+  <si>
+    <t>Stroh</t>
+  </si>
+  <si>
+    <t>rumratings.com</t>
+  </si>
+  <si>
+    <t>isokaato.com</t>
   </si>
 </sst>
 </file>
@@ -1532,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D380"/>
+  <dimension ref="A1:D400"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:D20"/>
+    <sheetView tabSelected="1" topLeftCell="A389" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D401" sqref="D401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6865,6 +6931,259 @@
         <v>382</v>
       </c>
     </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>383</v>
+      </c>
+      <c r="B381">
+        <v>22</v>
+      </c>
+      <c r="C381">
+        <v>5</v>
+      </c>
+      <c r="D381" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>384</v>
+      </c>
+      <c r="B382">
+        <v>29</v>
+      </c>
+      <c r="C382">
+        <v>95</v>
+      </c>
+      <c r="D382" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>385</v>
+      </c>
+      <c r="B383">
+        <v>48</v>
+      </c>
+      <c r="C383">
+        <v>5</v>
+      </c>
+      <c r="D383" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>386</v>
+      </c>
+      <c r="B384">
+        <v>54</v>
+      </c>
+      <c r="C384">
+        <v>16</v>
+      </c>
+      <c r="D384" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>387</v>
+      </c>
+      <c r="B385">
+        <v>47</v>
+      </c>
+      <c r="C385">
+        <v>11</v>
+      </c>
+      <c r="D385" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>388</v>
+      </c>
+      <c r="B386">
+        <v>48</v>
+      </c>
+      <c r="C386">
+        <v>9</v>
+      </c>
+      <c r="D386" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>389</v>
+      </c>
+      <c r="B387">
+        <v>20</v>
+      </c>
+      <c r="C387">
+        <v>1</v>
+      </c>
+      <c r="D387" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>390</v>
+      </c>
+      <c r="B388">
+        <v>30</v>
+      </c>
+      <c r="C388">
+        <v>1</v>
+      </c>
+      <c r="D388" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>391</v>
+      </c>
+      <c r="B389">
+        <v>49</v>
+      </c>
+      <c r="C389">
+        <v>31</v>
+      </c>
+      <c r="D389" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>392</v>
+      </c>
+      <c r="B390">
+        <v>48</v>
+      </c>
+      <c r="C390">
+        <v>5</v>
+      </c>
+      <c r="D390" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>393</v>
+      </c>
+      <c r="B391">
+        <v>29</v>
+      </c>
+      <c r="C391">
+        <v>95</v>
+      </c>
+      <c r="D391" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>394</v>
+      </c>
+      <c r="B392">
+        <v>52</v>
+      </c>
+      <c r="C392">
+        <v>25</v>
+      </c>
+      <c r="D392" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>397</v>
+      </c>
+      <c r="B395">
+        <v>63</v>
+      </c>
+      <c r="C395">
+        <v>4</v>
+      </c>
+      <c r="D395" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>398</v>
+      </c>
+      <c r="B396">
+        <v>47</v>
+      </c>
+      <c r="C396">
+        <v>24</v>
+      </c>
+      <c r="D396" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>400</v>
+      </c>
+      <c r="B398">
+        <v>76</v>
+      </c>
+      <c r="C398">
+        <v>285</v>
+      </c>
+      <c r="D398" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>401</v>
+      </c>
+      <c r="B399">
+        <v>48</v>
+      </c>
+      <c r="C399">
+        <v>117</v>
+      </c>
+      <c r="D399" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>402</v>
+      </c>
+      <c r="B400">
+        <v>39</v>
+      </c>
+      <c r="C400">
+        <v>32</v>
+      </c>
+      <c r="D400" t="s">
+        <v>403</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaned up frontend design
</commit_message>
<xml_diff>
--- a/assets/rumhowler_data.xlsx
+++ b/assets/rumhowler_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\OneDrive\Työpöytä\Programming projects\alko_app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E927FA-7B6D-4493-BBDE-DC01C7EC9267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF13093A-294E-45BC-97D9-3BAE38305D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="515">
   <si>
     <t>Rum</t>
   </si>
@@ -1235,6 +1235,336 @@
   </si>
   <si>
     <t>isokaato.com</t>
+  </si>
+  <si>
+    <t>Rum Nr. 7 Black muovipullo</t>
+  </si>
+  <si>
+    <t>Mount Gay Eclipse Navy Strength</t>
+  </si>
+  <si>
+    <t>Rivière du Mât Black Spiced</t>
+  </si>
+  <si>
+    <t>Havana Club Añejo Especial</t>
+  </si>
+  <si>
+    <t>Barracuda Caribbean White muovipullo</t>
+  </si>
+  <si>
+    <t>Bacardi Spiced</t>
+  </si>
+  <si>
+    <t>Bacardi Razz</t>
+  </si>
+  <si>
+    <t>Bacardi Limón</t>
+  </si>
+  <si>
+    <t>Captain Morgan</t>
+  </si>
+  <si>
+    <t>Havana Club Cuban Spiced</t>
+  </si>
+  <si>
+    <t>Bacardi Coconut</t>
+  </si>
+  <si>
+    <t>Angostura White Reserva</t>
+  </si>
+  <si>
+    <t>Diplomático Planas</t>
+  </si>
+  <si>
+    <t>Stroh 60 % muovipullo</t>
+  </si>
+  <si>
+    <t>Matusalem Solera 7</t>
+  </si>
+  <si>
+    <t>La Cruz Spiced muovipullo</t>
+  </si>
+  <si>
+    <t>Planteray Barbados Grande Reserve</t>
+  </si>
+  <si>
+    <t>Rivière du Mât Arrangé Vanille</t>
+  </si>
+  <si>
+    <t>Rivière du Mât Arrangé Ananas</t>
+  </si>
+  <si>
+    <t>Botran 8</t>
+  </si>
+  <si>
+    <t>Bush Rum Passionfruit &amp; Guava</t>
+  </si>
+  <si>
+    <t>Plantation Xaymaca Special Dry</t>
+  </si>
+  <si>
+    <t>Bacardi Reserva Ocho</t>
+  </si>
+  <si>
+    <t>Diplomático Mantuano</t>
+  </si>
+  <si>
+    <t>Westbourne Duppy Share White</t>
+  </si>
+  <si>
+    <t>Malecon Rare Proof Añejo 13 Años</t>
+  </si>
+  <si>
+    <t>The Duppy Share Aged</t>
+  </si>
+  <si>
+    <t>Chairman's Reserve White</t>
+  </si>
+  <si>
+    <t>Naud Ron Venezuela 12 Años</t>
+  </si>
+  <si>
+    <t>Island Signature Anacaona Gran Reserva Rum</t>
+  </si>
+  <si>
+    <t>Island Signature Turquoise Bay Amber Rum</t>
+  </si>
+  <si>
+    <t>Island Signature Tierra Madre</t>
+  </si>
+  <si>
+    <t>Island Signature Yellow Snake Amber Rum</t>
+  </si>
+  <si>
+    <t>Planteray Isle of Fiji</t>
+  </si>
+  <si>
+    <t>Canerock</t>
+  </si>
+  <si>
+    <t>Mulata Carta Blanca 3 Años</t>
+  </si>
+  <si>
+    <t>E.T.51 Premium Rum</t>
+  </si>
+  <si>
+    <t>The Demon's Share 3 Year Old</t>
+  </si>
+  <si>
+    <t>Come Hell Or High Water Spiced</t>
+  </si>
+  <si>
+    <t>Bayou Pink</t>
+  </si>
+  <si>
+    <t>Mezan Chiriqui</t>
+  </si>
+  <si>
+    <t>By the Dutch Batavia Arrack Indonesia Rum</t>
+  </si>
+  <si>
+    <t>Pusser's Original</t>
+  </si>
+  <si>
+    <t>Equiano Light Rum</t>
+  </si>
+  <si>
+    <t>Planteray Cut &amp; Dry Coconut</t>
+  </si>
+  <si>
+    <t>The Demons Share 6 Years Old</t>
+  </si>
+  <si>
+    <t>Compagnie Des Indes Jamaica 5 Year Old</t>
+  </si>
+  <si>
+    <t>Ron Tabú Ronmiel</t>
+  </si>
+  <si>
+    <t>Motörhead Premium Dark Rum</t>
+  </si>
+  <si>
+    <t>Captain Morgan Tiki</t>
+  </si>
+  <si>
+    <t>Discarded Banana Peel</t>
+  </si>
+  <si>
+    <t>Ron Aldea Single Estate Eco Rhum 2019</t>
+  </si>
+  <si>
+    <t>Naud Ron Panamá 15 Años</t>
+  </si>
+  <si>
+    <t>Pusser's Rum Coronation Reserve</t>
+  </si>
+  <si>
+    <t>Bumbu</t>
+  </si>
+  <si>
+    <t>rum-x.com</t>
+  </si>
+  <si>
+    <t>therumbarrel.co.uk</t>
+  </si>
+  <si>
+    <t>Hell Or High Water Rum Reserva</t>
+  </si>
+  <si>
+    <t>Hell Or High Water Reserva Honey &amp; Orange</t>
+  </si>
+  <si>
+    <t>Planteray Sealander</t>
+  </si>
+  <si>
+    <t>Bodegas Papiamento Caribbean Carnival</t>
+  </si>
+  <si>
+    <t>Readers´Rum Preface</t>
+  </si>
+  <si>
+    <t>Compañero Panama Extra Añejo</t>
+  </si>
+  <si>
+    <t>Hee Joy VSOP Dominican Rum</t>
+  </si>
+  <si>
+    <t>Hee Joy VSOP Rum Jamaica</t>
+  </si>
+  <si>
+    <t>After Rum</t>
+  </si>
+  <si>
+    <t>Come Hell Or High Water Rum XO</t>
+  </si>
+  <si>
+    <t>Relicario Ron Dominicano</t>
+  </si>
+  <si>
+    <t>Plantation Venezuela Vintage 2010</t>
+  </si>
+  <si>
+    <t>Martes Santo Añejo</t>
+  </si>
+  <si>
+    <t>Renegade Old Bacolet Pre-Cask Single Farm Rum 2020</t>
+  </si>
+  <si>
+    <t>Plantation Barbados Vintage 2013</t>
+  </si>
+  <si>
+    <t>Planteray Barbados 20th Anniversary XO</t>
+  </si>
+  <si>
+    <t>Rhum J.M. Terroir Volcanique Rhum Vieux Agricole</t>
+  </si>
+  <si>
+    <t>Plantation Panama Vintage 2010</t>
+  </si>
+  <si>
+    <t>Planteray Single Cask Paraguay 2019 Kyrö Rye Whisky Cask Finish</t>
+  </si>
+  <si>
+    <t>Planteray Single Cask Fiji Islands 2019 Coffee Liqueur Cask Finish</t>
+  </si>
+  <si>
+    <t>Bumbu XO</t>
+  </si>
+  <si>
+    <t>Equiano Original Rum</t>
+  </si>
+  <si>
+    <t>The Real McCoy 12 Year Old</t>
+  </si>
+  <si>
+    <t>Plantation Barbados Vintage 2007</t>
+  </si>
+  <si>
+    <t>Casa Elemental Ron Blanco Artesanal</t>
+  </si>
+  <si>
+    <t>Ron Matusalem Gran Reserva Solera 15</t>
+  </si>
+  <si>
+    <t>Rammstein Rum</t>
+  </si>
+  <si>
+    <t>Caña de Emperador 16 Year Old Guyana Rum</t>
+  </si>
+  <si>
+    <t>Botran Solera 1893</t>
+  </si>
+  <si>
+    <t>Banditti Club</t>
+  </si>
+  <si>
+    <t>Readers' Rum Chapter One</t>
+  </si>
+  <si>
+    <t>Diplomático Selección de Familia</t>
+  </si>
+  <si>
+    <t>Bristol Spirits Trinidad 8 Years Old</t>
+  </si>
+  <si>
+    <t>Centenario Ron Fundación 20 Aniversario</t>
+  </si>
+  <si>
+    <t>Mount Gay XO Triple Cask Blend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planteray Barbados 20th Anniversary XO Pedro Ximenez Cask Finish </t>
+  </si>
+  <si>
+    <t>Dictador 12 Years Icon Reserve</t>
+  </si>
+  <si>
+    <t>Kalevala Runoi Rum</t>
+  </si>
+  <si>
+    <t>Brugal Colección Visionaria Edición 02</t>
+  </si>
+  <si>
+    <t>Dictador Icon Reserve 20 Year Old</t>
+  </si>
+  <si>
+    <t>Ron Matusalem 23 Gran Reserva</t>
+  </si>
+  <si>
+    <t>Saint James Single Cask Rhum Vieux Agricole 1999</t>
+  </si>
+  <si>
+    <t>Mount Gay XO The Peat Smoke Expression</t>
+  </si>
+  <si>
+    <t>Brugal Maestro Reserva</t>
+  </si>
+  <si>
+    <t>Havana Club Añejo 15 Años Gran Reserva</t>
+  </si>
+  <si>
+    <t>Mount Gay Single Estate Series Release 01</t>
+  </si>
+  <si>
+    <t>Mount Gay Single Estate Series Release 24_02</t>
+  </si>
+  <si>
+    <t>Havana Club Maximo</t>
+  </si>
+  <si>
+    <t>amazon.co.uk</t>
+  </si>
+  <si>
+    <t>reddit.com/r/rum</t>
+  </si>
+  <si>
+    <t>rhumattitude.com</t>
+  </si>
+  <si>
+    <t>excellencerhum.com</t>
+  </si>
+  <si>
+    <t>masterofmalt.com</t>
   </si>
 </sst>
 </file>
@@ -1598,10 +1928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D400"/>
+  <dimension ref="A1:D504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A389" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D401" sqref="D401"/>
+    <sheetView tabSelected="1" topLeftCell="A490" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C506" sqref="C506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,13 +2744,13 @@
         <v>372</v>
       </c>
       <c r="B58">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>591</v>
       </c>
       <c r="D58" t="s">
-        <v>382</v>
+        <v>403</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -7181,6 +7511,1414 @@
         <v>32</v>
       </c>
       <c r="D400" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>405</v>
+      </c>
+      <c r="B401">
+        <v>13</v>
+      </c>
+      <c r="C401">
+        <v>4</v>
+      </c>
+      <c r="D401" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>406</v>
+      </c>
+      <c r="B402">
+        <v>63</v>
+      </c>
+      <c r="C402">
+        <v>11</v>
+      </c>
+      <c r="D402" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>407</v>
+      </c>
+      <c r="B403">
+        <v>65</v>
+      </c>
+      <c r="C403">
+        <v>21</v>
+      </c>
+      <c r="D403" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>408</v>
+      </c>
+      <c r="B404">
+        <v>60</v>
+      </c>
+      <c r="C404">
+        <v>447</v>
+      </c>
+      <c r="D404" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>409</v>
+      </c>
+      <c r="B405">
+        <v>27</v>
+      </c>
+      <c r="C405">
+        <v>7</v>
+      </c>
+      <c r="D405" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>410</v>
+      </c>
+      <c r="B406">
+        <v>50</v>
+      </c>
+      <c r="C406">
+        <v>99</v>
+      </c>
+      <c r="D406" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>411</v>
+      </c>
+      <c r="B407">
+        <v>32</v>
+      </c>
+      <c r="C407">
+        <v>88</v>
+      </c>
+      <c r="D407" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>412</v>
+      </c>
+      <c r="B408">
+        <v>35</v>
+      </c>
+      <c r="C408">
+        <v>128</v>
+      </c>
+      <c r="D408" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>413</v>
+      </c>
+      <c r="B409">
+        <v>42</v>
+      </c>
+      <c r="C409">
+        <v>591</v>
+      </c>
+      <c r="D409" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>414</v>
+      </c>
+      <c r="B410">
+        <v>45</v>
+      </c>
+      <c r="C410">
+        <v>14</v>
+      </c>
+      <c r="D410" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>416</v>
+      </c>
+      <c r="B411">
+        <v>59</v>
+      </c>
+      <c r="C411">
+        <v>21</v>
+      </c>
+      <c r="D411" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>415</v>
+      </c>
+      <c r="B412">
+        <v>54</v>
+      </c>
+      <c r="C412">
+        <v>49</v>
+      </c>
+      <c r="D412" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>417</v>
+      </c>
+      <c r="B413">
+        <v>60</v>
+      </c>
+      <c r="C413">
+        <v>91</v>
+      </c>
+      <c r="D413" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>418</v>
+      </c>
+      <c r="B414">
+        <v>30</v>
+      </c>
+      <c r="C414">
+        <v>24</v>
+      </c>
+      <c r="D414" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>419</v>
+      </c>
+      <c r="B415">
+        <v>60</v>
+      </c>
+      <c r="C415">
+        <v>52</v>
+      </c>
+      <c r="D415" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>421</v>
+      </c>
+      <c r="B417">
+        <v>65</v>
+      </c>
+      <c r="C417">
+        <v>312</v>
+      </c>
+      <c r="D417" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>422</v>
+      </c>
+      <c r="B418">
+        <v>52</v>
+      </c>
+      <c r="C418">
+        <v>5</v>
+      </c>
+      <c r="D418" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>423</v>
+      </c>
+      <c r="B419">
+        <v>61</v>
+      </c>
+      <c r="C419">
+        <v>9</v>
+      </c>
+      <c r="D419" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>424</v>
+      </c>
+      <c r="B420">
+        <v>56</v>
+      </c>
+      <c r="C420">
+        <v>21</v>
+      </c>
+      <c r="D420" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>425</v>
+      </c>
+      <c r="B421">
+        <v>69</v>
+      </c>
+      <c r="C421">
+        <v>1</v>
+      </c>
+      <c r="D421" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>426</v>
+      </c>
+      <c r="B422">
+        <v>66</v>
+      </c>
+      <c r="C422">
+        <v>240</v>
+      </c>
+      <c r="D422" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>427</v>
+      </c>
+      <c r="B423">
+        <v>62</v>
+      </c>
+      <c r="C423">
+        <v>143</v>
+      </c>
+      <c r="D423" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>428</v>
+      </c>
+      <c r="B424">
+        <v>65</v>
+      </c>
+      <c r="C424">
+        <v>398</v>
+      </c>
+      <c r="D424" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>429</v>
+      </c>
+      <c r="B425">
+        <v>79</v>
+      </c>
+      <c r="C425">
+        <v>17</v>
+      </c>
+      <c r="D425" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>430</v>
+      </c>
+      <c r="B426">
+        <v>76</v>
+      </c>
+      <c r="C426">
+        <v>8</v>
+      </c>
+      <c r="D426" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>431</v>
+      </c>
+      <c r="B427">
+        <v>64</v>
+      </c>
+      <c r="C427">
+        <v>127</v>
+      </c>
+      <c r="D427" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>432</v>
+      </c>
+      <c r="B428">
+        <v>67</v>
+      </c>
+      <c r="C428">
+        <v>10</v>
+      </c>
+      <c r="D428" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>433</v>
+      </c>
+      <c r="B429">
+        <v>65</v>
+      </c>
+      <c r="C429">
+        <v>3</v>
+      </c>
+      <c r="D429" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>428</v>
+      </c>
+      <c r="B430">
+        <v>65</v>
+      </c>
+      <c r="C430">
+        <v>398</v>
+      </c>
+      <c r="D430" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>434</v>
+      </c>
+      <c r="B431">
+        <v>56</v>
+      </c>
+      <c r="C431">
+        <v>6</v>
+      </c>
+      <c r="D431" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>435</v>
+      </c>
+      <c r="B432">
+        <v>69</v>
+      </c>
+      <c r="C432">
+        <v>33</v>
+      </c>
+      <c r="D432" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>436</v>
+      </c>
+      <c r="B433">
+        <v>55</v>
+      </c>
+      <c r="C433">
+        <v>3</v>
+      </c>
+      <c r="D433" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>437</v>
+      </c>
+      <c r="B434">
+        <v>52</v>
+      </c>
+      <c r="C434">
+        <v>14</v>
+      </c>
+      <c r="D434" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>438</v>
+      </c>
+      <c r="B435">
+        <v>66</v>
+      </c>
+      <c r="C435">
+        <v>154</v>
+      </c>
+      <c r="D435" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>439</v>
+      </c>
+      <c r="B436">
+        <v>58</v>
+      </c>
+      <c r="C436">
+        <v>73</v>
+      </c>
+      <c r="D436" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>440</v>
+      </c>
+      <c r="B437">
+        <v>70</v>
+      </c>
+      <c r="C437">
+        <v>3</v>
+      </c>
+      <c r="D437" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>441</v>
+      </c>
+      <c r="B438">
+        <v>55</v>
+      </c>
+      <c r="C438">
+        <v>2</v>
+      </c>
+      <c r="D438" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>442</v>
+      </c>
+      <c r="B439">
+        <v>50</v>
+      </c>
+      <c r="C439">
+        <v>12</v>
+      </c>
+      <c r="D439" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>443</v>
+      </c>
+      <c r="B440">
+        <v>30</v>
+      </c>
+      <c r="C440">
+        <v>4</v>
+      </c>
+      <c r="D440" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>444</v>
+      </c>
+      <c r="B441">
+        <v>46</v>
+      </c>
+      <c r="C441">
+        <v>8</v>
+      </c>
+      <c r="D441" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>445</v>
+      </c>
+      <c r="B442">
+        <v>52</v>
+      </c>
+      <c r="C442">
+        <v>13</v>
+      </c>
+      <c r="D442" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>446</v>
+      </c>
+      <c r="B443">
+        <v>84.5</v>
+      </c>
+      <c r="C443">
+        <v>1</v>
+      </c>
+      <c r="D443" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>447</v>
+      </c>
+      <c r="B444">
+        <v>67</v>
+      </c>
+      <c r="C444">
+        <v>461</v>
+      </c>
+      <c r="D444" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>448</v>
+      </c>
+      <c r="B445">
+        <v>58</v>
+      </c>
+      <c r="C445">
+        <v>5</v>
+      </c>
+      <c r="D445" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>449</v>
+      </c>
+      <c r="B446">
+        <v>76</v>
+      </c>
+      <c r="C446">
+        <v>17</v>
+      </c>
+      <c r="D446" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>450</v>
+      </c>
+      <c r="B447">
+        <v>53</v>
+      </c>
+      <c r="C447">
+        <v>75</v>
+      </c>
+      <c r="D447" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>451</v>
+      </c>
+      <c r="B448">
+        <v>62</v>
+      </c>
+      <c r="C448">
+        <v>6</v>
+      </c>
+      <c r="D448" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>453</v>
+      </c>
+      <c r="B450">
+        <v>67</v>
+      </c>
+      <c r="C450">
+        <v>46</v>
+      </c>
+      <c r="D450" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>454</v>
+      </c>
+      <c r="B451">
+        <v>28</v>
+      </c>
+      <c r="C451">
+        <v>29</v>
+      </c>
+      <c r="D451" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>455</v>
+      </c>
+      <c r="B452">
+        <v>69</v>
+      </c>
+      <c r="C452">
+        <v>21</v>
+      </c>
+      <c r="D452" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>456</v>
+      </c>
+      <c r="B453">
+        <v>62</v>
+      </c>
+      <c r="C453">
+        <v>10</v>
+      </c>
+      <c r="D453" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>457</v>
+      </c>
+      <c r="B454">
+        <v>70</v>
+      </c>
+      <c r="C454">
+        <v>27</v>
+      </c>
+      <c r="D454" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>458</v>
+      </c>
+      <c r="B455">
+        <v>77</v>
+      </c>
+      <c r="C455">
+        <v>11</v>
+      </c>
+      <c r="D455" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>459</v>
+      </c>
+      <c r="B456">
+        <v>63</v>
+      </c>
+      <c r="C456">
+        <v>958</v>
+      </c>
+      <c r="D456" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>462</v>
+      </c>
+      <c r="B457">
+        <v>60</v>
+      </c>
+      <c r="C457">
+        <v>1</v>
+      </c>
+      <c r="D457" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>463</v>
+      </c>
+      <c r="B458">
+        <v>92</v>
+      </c>
+      <c r="C458">
+        <v>9</v>
+      </c>
+      <c r="D458" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>464</v>
+      </c>
+      <c r="B459">
+        <v>68</v>
+      </c>
+      <c r="C459">
+        <v>30</v>
+      </c>
+      <c r="D459" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>465</v>
+      </c>
+      <c r="B460">
+        <v>55</v>
+      </c>
+      <c r="C460">
+        <v>1</v>
+      </c>
+      <c r="D460" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>466</v>
+      </c>
+      <c r="D461" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>467</v>
+      </c>
+      <c r="B462">
+        <v>73</v>
+      </c>
+      <c r="C462">
+        <v>131</v>
+      </c>
+      <c r="D462" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>468</v>
+      </c>
+      <c r="D463" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>469</v>
+      </c>
+      <c r="B464">
+        <v>80</v>
+      </c>
+      <c r="C464">
+        <v>1</v>
+      </c>
+      <c r="D464" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>470</v>
+      </c>
+      <c r="B465">
+        <v>96</v>
+      </c>
+      <c r="C465">
+        <v>375</v>
+      </c>
+      <c r="D465" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>471</v>
+      </c>
+      <c r="B466">
+        <v>69</v>
+      </c>
+      <c r="C466">
+        <v>17</v>
+      </c>
+      <c r="D466" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>472</v>
+      </c>
+      <c r="B467">
+        <v>80</v>
+      </c>
+      <c r="C467">
+        <v>3</v>
+      </c>
+      <c r="D467" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>473</v>
+      </c>
+      <c r="B468">
+        <v>76</v>
+      </c>
+      <c r="C468">
+        <v>12</v>
+      </c>
+      <c r="D468" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>474</v>
+      </c>
+      <c r="D469" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>475</v>
+      </c>
+      <c r="B470">
+        <v>40</v>
+      </c>
+      <c r="C470">
+        <v>2</v>
+      </c>
+      <c r="D470" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>476</v>
+      </c>
+      <c r="B471">
+        <v>81</v>
+      </c>
+      <c r="C471">
+        <v>8</v>
+      </c>
+      <c r="D471" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>477</v>
+      </c>
+      <c r="B472">
+        <v>84</v>
+      </c>
+      <c r="C472">
+        <v>1933</v>
+      </c>
+      <c r="D472" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>478</v>
+      </c>
+      <c r="B473">
+        <v>67</v>
+      </c>
+      <c r="C473">
+        <v>47</v>
+      </c>
+      <c r="D473" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>479</v>
+      </c>
+      <c r="B474">
+        <v>67</v>
+      </c>
+      <c r="C474">
+        <v>3</v>
+      </c>
+      <c r="D474" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>480</v>
+      </c>
+      <c r="B475">
+        <v>65</v>
+      </c>
+      <c r="C475">
+        <v>2</v>
+      </c>
+      <c r="D475" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>481</v>
+      </c>
+      <c r="B476">
+        <v>73</v>
+      </c>
+      <c r="C476">
+        <v>3</v>
+      </c>
+      <c r="D476" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>482</v>
+      </c>
+      <c r="B477">
+        <v>71</v>
+      </c>
+      <c r="C477">
+        <v>306</v>
+      </c>
+      <c r="D477" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>483</v>
+      </c>
+      <c r="B478">
+        <v>76</v>
+      </c>
+      <c r="C478">
+        <v>105</v>
+      </c>
+      <c r="D478" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>484</v>
+      </c>
+      <c r="B479">
+        <v>76</v>
+      </c>
+      <c r="C479">
+        <v>188</v>
+      </c>
+      <c r="D479" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>485</v>
+      </c>
+      <c r="B480">
+        <v>81</v>
+      </c>
+      <c r="C480">
+        <v>75</v>
+      </c>
+      <c r="D480" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>486</v>
+      </c>
+      <c r="D481" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>487</v>
+      </c>
+      <c r="B482">
+        <v>64</v>
+      </c>
+      <c r="C482">
+        <v>713</v>
+      </c>
+      <c r="D482" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>488</v>
+      </c>
+      <c r="B483">
+        <v>72</v>
+      </c>
+      <c r="C483">
+        <v>55</v>
+      </c>
+      <c r="D483" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>489</v>
+      </c>
+      <c r="B484">
+        <v>75</v>
+      </c>
+      <c r="C484">
+        <v>3</v>
+      </c>
+      <c r="D484" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>490</v>
+      </c>
+      <c r="B485">
+        <v>70</v>
+      </c>
+      <c r="C485">
+        <v>225</v>
+      </c>
+      <c r="D485" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>491</v>
+      </c>
+      <c r="B486">
+        <v>80</v>
+      </c>
+      <c r="C486">
+        <v>22</v>
+      </c>
+      <c r="D486" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>492</v>
+      </c>
+      <c r="D487" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>493</v>
+      </c>
+      <c r="B488">
+        <v>81</v>
+      </c>
+      <c r="C488">
+        <v>145</v>
+      </c>
+      <c r="D488" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>494</v>
+      </c>
+      <c r="B489">
+        <v>87</v>
+      </c>
+      <c r="C489">
+        <v>3</v>
+      </c>
+      <c r="D489" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>495</v>
+      </c>
+      <c r="B490">
+        <v>82</v>
+      </c>
+      <c r="C490">
+        <v>385</v>
+      </c>
+      <c r="D490" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>496</v>
+      </c>
+      <c r="B491">
+        <v>80</v>
+      </c>
+      <c r="C491">
+        <v>143</v>
+      </c>
+      <c r="D491" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>497</v>
+      </c>
+      <c r="B492">
+        <v>84</v>
+      </c>
+      <c r="C492">
+        <v>1933</v>
+      </c>
+      <c r="D492" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>498</v>
+      </c>
+      <c r="B493">
+        <v>69</v>
+      </c>
+      <c r="C493">
+        <v>483</v>
+      </c>
+      <c r="D493" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>499</v>
+      </c>
+      <c r="B494">
+        <v>80</v>
+      </c>
+      <c r="C494">
+        <v>3</v>
+      </c>
+      <c r="D494" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>500</v>
+      </c>
+      <c r="B495">
+        <v>65</v>
+      </c>
+      <c r="C495">
+        <v>6</v>
+      </c>
+      <c r="D495" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>501</v>
+      </c>
+      <c r="B496">
+        <v>74</v>
+      </c>
+      <c r="C496">
+        <v>418</v>
+      </c>
+      <c r="D496" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>502</v>
+      </c>
+      <c r="B497">
+        <v>72</v>
+      </c>
+      <c r="C497">
+        <v>229</v>
+      </c>
+      <c r="D497" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>503</v>
+      </c>
+      <c r="B498">
+        <v>80</v>
+      </c>
+      <c r="C498">
+        <v>1</v>
+      </c>
+      <c r="D498" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>504</v>
+      </c>
+      <c r="B499">
+        <v>71</v>
+      </c>
+      <c r="C499">
+        <v>13</v>
+      </c>
+      <c r="D499" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>505</v>
+      </c>
+      <c r="B500">
+        <v>71</v>
+      </c>
+      <c r="C500">
+        <v>7</v>
+      </c>
+      <c r="D500" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>506</v>
+      </c>
+      <c r="B501">
+        <v>79</v>
+      </c>
+      <c r="C501">
+        <v>88</v>
+      </c>
+      <c r="D501" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>507</v>
+      </c>
+      <c r="B502">
+        <v>80</v>
+      </c>
+      <c r="C502">
+        <v>2</v>
+      </c>
+      <c r="D502" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>508</v>
+      </c>
+      <c r="B503">
+        <v>82</v>
+      </c>
+      <c r="C503">
+        <v>20</v>
+      </c>
+      <c r="D503" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>509</v>
+      </c>
+      <c r="B504">
+        <v>88</v>
+      </c>
+      <c r="C504">
+        <v>18</v>
+      </c>
+      <c r="D504" t="s">
         <v>403</v>
       </c>
     </row>

</xml_diff>